<commit_message>
Updated Risk Register with owners of risks for risks related to a single WP
</commit_message>
<xml_diff>
--- a/Work Packages/WP1 Management/Risks/PaNOSC Risk Register.xlsx
+++ b/Work Packages/WP1 Management/Risks/PaNOSC Risk Register.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
   <si>
     <t>#</t>
   </si>
@@ -297,6 +297,30 @@
   </si>
   <si>
     <t>Information from Project stage</t>
+  </si>
+  <si>
+    <t>Andy Gotz</t>
+  </si>
+  <si>
+    <t>Tobias Richter</t>
+  </si>
+  <si>
+    <t>Hans Fangohr</t>
+  </si>
+  <si>
+    <t>Carsten Fortmann-Grote</t>
+  </si>
+  <si>
+    <t>Jean-François Perrin</t>
+  </si>
+  <si>
+    <t>Roberto Pugliese</t>
+  </si>
+  <si>
+    <t>Thomas Rod</t>
+  </si>
+  <si>
+    <t>Nicoletta Carboni</t>
   </si>
 </sst>
 </file>
@@ -402,9 +426,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -414,9 +435,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -424,104 +442,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -573,7 +504,86 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -595,18 +605,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:M34" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:M34" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A2:M34"/>
   <tableColumns count="13">
     <tableColumn id="1" name="#"/>
     <tableColumn id="2" name="Risk Name"/>
-    <tableColumn id="3" name="Risk Description" dataDxfId="11"/>
+    <tableColumn id="3" name="Risk Description" dataDxfId="4"/>
     <tableColumn id="4" name="WP involved"/>
     <tableColumn id="5" name="Probability"/>
-    <tableColumn id="8" name="Initial mitigation measure" dataDxfId="0"/>
-    <tableColumn id="15" name="New Probability" dataDxfId="1"/>
-    <tableColumn id="14" name="Impact" dataDxfId="10"/>
-    <tableColumn id="13" name="Assessment" dataDxfId="9">
+    <tableColumn id="8" name="Initial mitigation measure" dataDxfId="3"/>
+    <tableColumn id="15" name="New Probability" dataDxfId="2"/>
+    <tableColumn id="14" name="Impact" dataDxfId="1"/>
+    <tableColumn id="13" name="Assessment" dataDxfId="0">
       <calculatedColumnFormula>IF(G3="Unlikely",IF(H3="Minor","Low","Medium"),
 IF(G3="Moderate",IF(H3="Major","High","Medium"),
 IF(G3="Very Likely",IF(H3="Minor","Medium",
@@ -911,7 +921,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +931,7 @@
     <col min="3" max="3" width="35.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="9" customWidth="1"/>
     <col min="7" max="7" width="13" style="3" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" style="3" customWidth="1"/>
@@ -932,61 +942,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1003,24 +1013,20 @@
       <c r="D3" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="2" t="str">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="b">
         <f t="shared" ref="I3:I34" si="0">IF(G3="Unlikely",IF(H3="Minor","Low","Medium"),
 IF(G3="Moderate",IF(H3="Major","High","Medium"),
 IF(G3="Very Likely",IF(H3="Minor","Medium",
 IF(H3="Moderate","High","Very High")))))</f>
-        <v>Medium</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
@@ -1036,21 +1042,17 @@
       <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
@@ -1066,21 +1068,17 @@
       <c r="D5" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>High</v>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
@@ -1096,21 +1094,20 @@
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="51.75" x14ac:dyDescent="0.25">
@@ -1126,21 +1123,20 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
@@ -1156,21 +1152,20 @@
       <c r="D8">
         <v>3</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="60.75" x14ac:dyDescent="0.25">
@@ -1186,21 +1181,20 @@
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
@@ -1216,21 +1210,20 @@
       <c r="D10">
         <v>4</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="60.75" x14ac:dyDescent="0.25">
@@ -1246,21 +1239,20 @@
       <c r="D11">
         <v>4</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
@@ -1276,21 +1268,20 @@
       <c r="D12">
         <v>5</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
@@ -1306,21 +1297,17 @@
       <c r="D13" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
@@ -1336,21 +1323,17 @@
       <c r="D14" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="39" x14ac:dyDescent="0.25">
@@ -1366,21 +1349,20 @@
       <c r="D15">
         <v>5</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1396,24 +1378,23 @@
       <c r="D16">
         <v>6</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1426,24 +1407,23 @@
       <c r="D17">
         <v>6</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1456,24 +1436,23 @@
       <c r="D18">
         <v>7</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="84.75" x14ac:dyDescent="0.25">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="84.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1486,24 +1465,23 @@
       <c r="D19">
         <v>7</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Low</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1516,24 +1494,23 @@
       <c r="D20">
         <v>7</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1546,24 +1523,23 @@
       <c r="D21">
         <v>7</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>High</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1576,24 +1552,23 @@
       <c r="D22">
         <v>8</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1606,24 +1581,20 @@
       <c r="D23" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1636,24 +1607,20 @@
       <c r="D24" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="84.75" x14ac:dyDescent="0.25">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="84.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1666,24 +1633,23 @@
       <c r="D25">
         <v>9</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1696,24 +1662,23 @@
       <c r="D26">
         <v>9</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="132.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="132.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1723,28 +1688,27 @@
       <c r="D27">
         <v>9</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Medium</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="F28" s="10"/>
+      <c r="F28" s="8"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="b">
@@ -1752,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1763,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1774,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1785,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1824,16 +1788,16 @@
     <mergeCell ref="G1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:I1048576">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Risk register. Template for PMC agenda and summary notes 03/07/2019
</commit_message>
<xml_diff>
--- a/Work Packages/WP1 Management/Risks/PaNOSC Risk Register.xlsx
+++ b/Work Packages/WP1 Management/Risks/PaNOSC Risk Register.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
   <si>
     <t>#</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Compute resources not available</t>
   </si>
   <si>
-    <t>Staff not recruited</t>
-  </si>
-  <si>
     <t>EOSC delays</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>Apply for HPC resources, e.g.</t>
   </si>
   <si>
-    <t>PRACE preliminary access</t>
-  </si>
-  <si>
     <t>Start recruitment as early as possible.</t>
   </si>
   <si>
@@ -321,6 +315,12 @@
   </si>
   <si>
     <t>Nicoletta Carboni</t>
+  </si>
+  <si>
+    <t>Delay in staff recruitment</t>
+  </si>
+  <si>
+    <t>EGI to advertise vacancies for us</t>
   </si>
 </sst>
 </file>
@@ -921,13 +921,13 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
@@ -943,7 +943,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -951,7 +951,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="G1" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
@@ -979,7 +979,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>4</v>
@@ -1011,22 +1011,26 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="b">
+        <v>60</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I34" si="0">IF(G3="Unlikely",IF(H3="Minor","Low","Medium"),
 IF(G3="Moderate",IF(H3="Major","High","Medium"),
 IF(G3="Very Likely",IF(H3="Minor","Medium",
 IF(H3="Moderate","High","Very High")))))</f>
-        <v>0</v>
+        <v>Medium</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
@@ -1040,19 +1044,23 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Medium</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
@@ -1066,19 +1074,23 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Medium</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
@@ -1095,10 +1107,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1107,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="51.75" x14ac:dyDescent="0.25">
@@ -1124,10 +1136,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1136,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
@@ -1153,10 +1165,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1165,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="60.75" x14ac:dyDescent="0.25">
@@ -1182,10 +1194,10 @@
         <v>3</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1194,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
@@ -1211,10 +1223,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1223,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="60.75" x14ac:dyDescent="0.25">
@@ -1240,10 +1252,10 @@
         <v>4</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1252,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
@@ -1269,10 +1281,10 @@
         <v>5</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1281,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
@@ -1295,13 +1307,13 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1321,13 +1333,13 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1350,10 +1362,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1362,15 +1374,15 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>25</v>
@@ -1379,19 +1391,26 @@
         <v>6</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>High</v>
+      </c>
+      <c r="J16" t="s">
+        <v>101</v>
       </c>
       <c r="K16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
@@ -1399,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>26</v>
@@ -1408,10 +1427,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1420,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -1437,10 +1456,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1449,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="84.75" x14ac:dyDescent="0.25">
@@ -1466,10 +1485,10 @@
         <v>7</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1478,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="39" x14ac:dyDescent="0.25">
@@ -1486,7 +1505,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>29</v>
@@ -1495,10 +1514,10 @@
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1507,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1524,10 +1543,10 @@
         <v>7</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1536,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -1544,7 +1563,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>31</v>
@@ -1553,10 +1572,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1565,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
@@ -1579,13 +1598,13 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1605,13 +1624,13 @@
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1634,10 +1653,10 @@
         <v>9</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1646,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
@@ -1663,10 +1682,10 @@
         <v>9</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1675,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="132.75" x14ac:dyDescent="0.25">
@@ -1689,10 +1708,10 @@
         <v>9</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1701,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1829,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,36 +1859,48 @@
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>87</v>
       </c>
-      <c r="D4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>89</v>
       </c>
-      <c r="D6" t="s">
-        <v>91</v>
+      <c r="F6" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
risks updated with infor from Andy & Jean-Francois
</commit_message>
<xml_diff>
--- a/Work Packages/WP1 Management/Risks/PaNOSC Risk Register.xlsx
+++ b/Work Packages/WP1 Management/Risks/PaNOSC Risk Register.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="107">
   <si>
     <t>#</t>
   </si>
@@ -321,13 +321,28 @@
   </si>
   <si>
     <t>EGI to advertise vacancies for us</t>
+  </si>
+  <si>
+    <t>All partners think that adopting a common framework is highly likely</t>
+  </si>
+  <si>
+    <t>Assessment Formula</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>Very low</t>
+  </si>
+  <si>
+    <t>No clear plan from partner sites how they will implement the DP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,8 +387,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +427,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -417,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -448,11 +495,130 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -473,6 +639,99 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -553,37 +812,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -605,22 +833,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:M34" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:M34" totalsRowShown="0" headerRowDxfId="30">
   <autoFilter ref="A2:M34"/>
   <tableColumns count="13">
     <tableColumn id="1" name="#"/>
     <tableColumn id="2" name="Risk Name"/>
-    <tableColumn id="3" name="Risk Description" dataDxfId="4"/>
+    <tableColumn id="3" name="Risk Description" dataDxfId="29"/>
     <tableColumn id="4" name="WP involved"/>
     <tableColumn id="5" name="Probability"/>
-    <tableColumn id="8" name="Initial mitigation measure" dataDxfId="3"/>
-    <tableColumn id="15" name="New Probability" dataDxfId="2"/>
-    <tableColumn id="14" name="Impact" dataDxfId="1"/>
-    <tableColumn id="13" name="Assessment" dataDxfId="0">
-      <calculatedColumnFormula>IF(G3="Unlikely",IF(H3="Minor","Low","Medium"),
-IF(G3="Moderate",IF(H3="Major","High","Medium"),
-IF(G3="Very Likely",IF(H3="Minor","Medium",
-IF(H3="Moderate","High","Very High")))))</calculatedColumnFormula>
+    <tableColumn id="8" name="Initial mitigation measure" dataDxfId="28"/>
+    <tableColumn id="15" name="New Probability" dataDxfId="27"/>
+    <tableColumn id="14" name="Impact" dataDxfId="26"/>
+    <tableColumn id="13" name="Assessment" dataDxfId="13">
+      <calculatedColumnFormula>IF(G3="Unlikely",IF(H3="Minor","1 Very Low",IF(H3="Moderate","2 Low","3 Medium")),
+IF(G3="Moderate",IF(H3="Minor","2 Low",
+IF(H3="Moderate","3 Medium","4 High")),
+IF(G3="Very Likely",IF(H3="Minor","3 Medium",
+IF(H3="Moderate","4 High","5 Very High")))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="Comments"/>
     <tableColumn id="10" name="Owner"/>
@@ -920,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +1163,7 @@
     <col min="6" max="6" width="35.7109375" style="9" customWidth="1"/>
     <col min="7" max="7" width="13" style="3" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="3" customWidth="1"/>
     <col min="10" max="10" width="35.7109375" customWidth="1"/>
     <col min="11" max="11" width="21.42578125" customWidth="1"/>
     <col min="12" max="12" width="35.7109375" customWidth="1"/>
@@ -1026,8 +1255,17 @@
         <v>86</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I34" si="0">IF(G3="Unlikely",IF(H3="Minor","Low","Medium"),
-IF(G3="Moderate",IF(H3="Major","High","Medium"),
+        <f t="shared" ref="I3:I34" si="0">IF(G3="Unlikely",IF(H3="Minor","1 Very Low",IF(H3="Moderate","2 Low","3 Medium")),
+IF(G3="Moderate",IF(H3="Minor","2 Low",
+IF(H3="Moderate","3 Medium","4 High")),
+IF(G3="Very Likely",IF(H3="Minor","3 Medium",
+IF(H3="Moderate","4 High","5 Very High")))))</f>
+        <v>3 Medium</v>
+      </c>
+      <c r="J3" t="str">
+        <f>IF(G3="Unlikely",IF(H3="Minor","Very Low",IF(H3="Moderate","Low","Medium")),
+IF(G3="Moderate",IF(H3="Minor","Medium",
+IF(H3="Moderate","Medium","High")),
 IF(G3="Very Likely",IF(H3="Minor","Medium",
 IF(H3="Moderate","High","Very High")))))</f>
         <v>Medium</v>
@@ -1060,7 +1298,7 @@
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Medium</v>
+        <v>2 Low</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="48.75" x14ac:dyDescent="0.25">
@@ -1090,7 +1328,7 @@
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Medium</v>
+        <v>2 Low</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
@@ -1112,11 +1350,18 @@
       <c r="F6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>2 Low</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="K6" t="s">
         <v>92</v>
@@ -1141,11 +1386,18 @@
       <c r="F7" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>3 Medium</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="K7" t="s">
         <v>92</v>
@@ -1404,7 +1656,7 @@
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>High</v>
+        <v>4 High</v>
       </c>
       <c r="J16" t="s">
         <v>101</v>
@@ -1529,7 +1781,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1741,7 +1993,7 @@
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="3" t="b">
+      <c r="I29" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1752,7 +2004,7 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="3" t="b">
+      <c r="I30" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1763,7 +2015,7 @@
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="3" t="b">
+      <c r="I31" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1774,7 +2026,7 @@
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="3" t="b">
+      <c r="I32" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1785,7 +2037,7 @@
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="3" t="b">
+      <c r="I33" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1796,7 +2048,7 @@
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="3" t="b">
+      <c r="I34" s="2" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1807,17 +2059,22 @@
     <mergeCell ref="G1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:I1048576">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
-      <formula>"Low"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"2 Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
-      <formula>"Medium"</formula>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"3 Medium"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>"High"</formula>
+      <formula>"4 High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
-      <formula>"Very High"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"5 Very High"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"1 Very Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1848,29 +2105,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>85</v>
       </c>
@@ -1880,8 +2157,14 @@
       <c r="F4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -1889,10 +2172,28 @@
         <v>86</v>
       </c>
       <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="M5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>87</v>
       </c>
@@ -1900,10 +2201,119 @@
         <v>89</v>
       </c>
       <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
         <v>87</v>
       </c>
+      <c r="G10" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>